<commit_message>
combined results in excel file, changed main.py slightly to make it faster
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="460" yWindow="780" windowWidth="37840" windowHeight="20800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -627,11 +627,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="177413136"/>
-        <c:axId val="177414912"/>
+        <c:axId val="-1232095808"/>
+        <c:axId val="-1270022608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="177413136"/>
+        <c:axId val="-1232095808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177414912"/>
+        <c:crossAx val="-1270022608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -682,7 +682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177414912"/>
+        <c:axId val="-1270022608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,6 +758,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -788,7 +789,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177413136"/>
+        <c:crossAx val="-1232095808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1385,11 +1386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="183804048"/>
-        <c:axId val="177264288"/>
+        <c:axId val="-1190106304"/>
+        <c:axId val="-1190103824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="183804048"/>
+        <c:axId val="-1190106304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177264288"/>
+        <c:crossAx val="-1190103824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1440,7 +1441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177264288"/>
+        <c:axId val="-1190103824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183804048"/>
+        <c:crossAx val="-1190106304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1859,11 +1860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="66393712"/>
-        <c:axId val="219289952"/>
+        <c:axId val="-1190083168"/>
+        <c:axId val="-1190080416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66393712"/>
+        <c:axId val="-1190083168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219289952"/>
+        <c:crossAx val="-1190080416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219289952"/>
+        <c:axId val="-1190080416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,7 +1965,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66393712"/>
+        <c:crossAx val="-1190083168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2240,11 +2241,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="219886048"/>
-        <c:axId val="150623232"/>
+        <c:axId val="-1190059680"/>
+        <c:axId val="-1190056928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="219886048"/>
+        <c:axId val="-1190059680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2287,7 +2288,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150623232"/>
+        <c:crossAx val="-1190056928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2295,7 +2296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150623232"/>
+        <c:axId val="-1190056928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,7 +2346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219886048"/>
+        <c:crossAx val="-1190059680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2503,6 +2504,63 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$41:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$41:$G$56</c:f>
@@ -2571,16 +2629,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="146201904"/>
-        <c:axId val="146766624"/>
+        <c:axId val="-1190033568"/>
+        <c:axId val="-1190030816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146201904"/>
+        <c:axId val="-1190033568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2617,7 +2676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146766624"/>
+        <c:crossAx val="-1190030816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2625,7 +2684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146766624"/>
+        <c:axId val="-1190030816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2675,7 +2734,322 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146201904"/>
+        <c:crossAx val="-1190033568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.398722222222222"/>
+          <c:y val="0.0555555555555555"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conflicts </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$60:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$60:$G$67</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>205121.0425</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22273.3935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.2309999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.97299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.178999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1186887360"/>
+        <c:axId val="-1142146512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1186887360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1142146512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1142146512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1186887360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2924,6 +3298,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4989,6 +5403,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5569,15 +6499,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5604,10 +6534,10 @@
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5629,15 +6559,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5651,6 +6581,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5936,10 +6896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V51" sqref="V51"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59:G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7832,6 +8792,389 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>0.2</v>
+      </c>
+      <c r="B60" s="1">
+        <v>8.5044499999999896</v>
+      </c>
+      <c r="C60" s="1">
+        <v>73.403150000000039</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1986.9925000000001</v>
+      </c>
+      <c r="E60" s="1">
+        <v>99.9215999999996</v>
+      </c>
+      <c r="F60" s="1">
+        <v>335.58350000000002</v>
+      </c>
+      <c r="G60" s="1">
+        <v>205121.04250000001</v>
+      </c>
+      <c r="H60" s="1">
+        <v>13258.586999999949</v>
+      </c>
+      <c r="I60" s="1">
+        <v>17110.780999999901</v>
+      </c>
+      <c r="J60" s="1">
+        <v>12.1336999999999</v>
+      </c>
+      <c r="K60" s="1">
+        <v>20.99334999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f>A60+0.1</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.91954999999999854</v>
+      </c>
+      <c r="C61" s="1">
+        <v>30.0869</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1322.1709999999948</v>
+      </c>
+      <c r="E61" s="1">
+        <v>99.4117999999999</v>
+      </c>
+      <c r="F61" s="1">
+        <v>284.64349999999899</v>
+      </c>
+      <c r="G61" s="1">
+        <v>22273.393499999998</v>
+      </c>
+      <c r="H61" s="1">
+        <v>3606.6074999999951</v>
+      </c>
+      <c r="I61" s="1">
+        <v>4816.3490000000002</v>
+      </c>
+      <c r="J61" s="1">
+        <v>11.349549999999899</v>
+      </c>
+      <c r="K61" s="1">
+        <v>18.427299999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" ref="A62:A68" si="3">A61+0.1</f>
+        <v>0.4</v>
+      </c>
+      <c r="B62" s="1">
+        <v>3.9999999999999996E-4</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2.9390999999999803</v>
+      </c>
+      <c r="D62" s="1">
+        <v>113.541</v>
+      </c>
+      <c r="E62" s="1">
+        <v>99.770299999999949</v>
+      </c>
+      <c r="F62" s="1">
+        <v>40.891999999999953</v>
+      </c>
+      <c r="G62" s="1">
+        <v>101.23099999999951</v>
+      </c>
+      <c r="H62" s="1">
+        <v>21.750999999999948</v>
+      </c>
+      <c r="I62" s="1">
+        <v>959.88699999999994</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.75544999999999995</v>
+      </c>
+      <c r="K62" s="1">
+        <v>17.633600000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1.2829999999999901</v>
+      </c>
+      <c r="D63" s="1">
+        <v>17.268999999999849</v>
+      </c>
+      <c r="E63" s="1">
+        <v>99.898750000000092</v>
+      </c>
+      <c r="F63" s="1">
+        <v>114.05500000000001</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1.9729999999999901</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>822.5</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1">
+        <v>17.634049999999952</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.66374999999999851</v>
+      </c>
+      <c r="D64" s="1">
+        <v>6.9344999999999946</v>
+      </c>
+      <c r="E64" s="1">
+        <v>99.943649999999707</v>
+      </c>
+      <c r="F64" s="1">
+        <v>292.49349999999947</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.17899999999999949</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>537.5</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1">
+        <v>17.6924999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="B65" s="1">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="D65" s="1">
+        <v>2.3569999999999949</v>
+      </c>
+      <c r="E65" s="1">
+        <v>99.976049999999347</v>
+      </c>
+      <c r="F65" s="1">
+        <v>479.60699999999997</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1.9000000000000003E-2</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>234.5</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1">
+        <v>17.753099999999797</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>6.4750000000000002E-2</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.5475000000000001</v>
+      </c>
+      <c r="E66" s="1">
+        <v>99.993599999999248</v>
+      </c>
+      <c r="F66" s="1">
+        <v>585.27350000000001</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>64</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1">
+        <v>17.7871999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E67" s="1">
+        <v>99.999399999999241</v>
+      </c>
+      <c r="F67" s="1">
+        <v>621.27399999999898</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>6</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1">
+        <v>17.798799999999702</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>